<commit_message>
Added excel reading utility
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhils\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Music\MyOwnFramework_Nikhil\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650BD9EB-8FA9-4EED-A67C-FC596D35D9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B6F0F-7E5A-4DF8-9C8C-133D2706B6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Test005</t>
+  </si>
+  <si>
+    <t>expectedUser</t>
+  </si>
+  <si>
+    <t>webpageURL</t>
+  </si>
+  <si>
+    <t>webpageName</t>
   </si>
 </sst>
 </file>
@@ -84,8 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,68 +378,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>1234</v>
+      <c r="B7" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated VAX Framework code
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhils\Music\OwnFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6FCFA4-6500-4FF1-8BA9-8B95A3DD05B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3418FEA-7A40-44BE-BCCC-157014D64C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="WebPage" sheetId="2" r:id="rId2"/>
-    <sheet name="Views" sheetId="3" r:id="rId3"/>
-    <sheet name="Tours" sheetId="4" r:id="rId4"/>
+    <sheet name="logindetails" sheetId="1" r:id="rId1"/>
+    <sheet name="webpages" sheetId="2" r:id="rId2"/>
+    <sheet name="views" sheetId="3" r:id="rId3"/>
+    <sheet name="tours" sheetId="4" r:id="rId4"/>
+    <sheet name="vasalarms" sheetId="5" r:id="rId5"/>
+    <sheet name="vaxalarms" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>username</t>
   </si>
@@ -55,19 +57,220 @@
   </si>
   <si>
     <t>expectedUser</t>
+  </si>
+  <si>
+    <t>webpageName</t>
+  </si>
+  <si>
+    <t>webpageURL</t>
+  </si>
+  <si>
+    <t>1. Alibaba</t>
+  </si>
+  <si>
+    <t>2. NDTV</t>
+  </si>
+  <si>
+    <t>3. Vicon</t>
+  </si>
+  <si>
+    <t>4. ZeeNews</t>
+  </si>
+  <si>
+    <t>5. Selenium Dev</t>
+  </si>
+  <si>
+    <t>6. TestNG</t>
+  </si>
+  <si>
+    <t>7. Cemtrex Labs</t>
+  </si>
+  <si>
+    <t>http://www.alibaba.com</t>
+  </si>
+  <si>
+    <t>http://www.ndtv.com</t>
+  </si>
+  <si>
+    <t>http://www.zeenews.com</t>
+  </si>
+  <si>
+    <t>https://www.vicon.com/</t>
+  </si>
+  <si>
+    <t>https://www.selenium.dev/</t>
+  </si>
+  <si>
+    <t>https://testng.org/doc/</t>
+  </si>
+  <si>
+    <t>https://cemtrex.com/</t>
+  </si>
+  <si>
+    <t>vaxAlarmNames</t>
+  </si>
+  <si>
+    <t>additionalInformationMessage</t>
+  </si>
+  <si>
+    <t>1. Door Locked</t>
+  </si>
+  <si>
+    <t>2. Door Unlocked</t>
+  </si>
+  <si>
+    <t>3. Door Open</t>
+  </si>
+  <si>
+    <t>4. Door Close</t>
+  </si>
+  <si>
+    <t>5. Door Forced Open</t>
+  </si>
+  <si>
+    <t>6. Door Held Open</t>
+  </si>
+  <si>
+    <t>7. Door Override Enabled</t>
+  </si>
+  <si>
+    <t>8. Door Override Disabled</t>
+  </si>
+  <si>
+    <t>9. Door Override Auto resume</t>
+  </si>
+  <si>
+    <t>11. Access Granted - Pin</t>
+  </si>
+  <si>
+    <t>12. Access Granted - Master Priv.</t>
+  </si>
+  <si>
+    <t>13. Access Denied - Wrong time Zone.</t>
+  </si>
+  <si>
+    <t>14. Access Denied - No Privilege.</t>
+  </si>
+  <si>
+    <t>15. Access Denied - Invalid Card</t>
+  </si>
+  <si>
+    <t>16. Access Denied - Invalid Start Date</t>
+  </si>
+  <si>
+    <t>17. Access Denied - Invalid End Date</t>
+  </si>
+  <si>
+    <t>18. Access Denied - Invalid Security Level</t>
+  </si>
+  <si>
+    <t>19. Access Denied - Unknown Card Form</t>
+  </si>
+  <si>
+    <t>20. VAX Digital Input</t>
+  </si>
+  <si>
+    <t>10. Access Granted - Card</t>
+  </si>
+  <si>
+    <t>21. VAX Relay Output</t>
+  </si>
+  <si>
+    <t>22. Message- Door Locked</t>
+  </si>
+  <si>
+    <t>23. Message- Door Unlocked</t>
+  </si>
+  <si>
+    <t>24. Message-Door Overridde Enable</t>
+  </si>
+  <si>
+    <t>25. Message-Door Open</t>
+  </si>
+  <si>
+    <t>26. Message-Door Closed</t>
+  </si>
+  <si>
+    <t>27. Message-Door Forced Open</t>
+  </si>
+  <si>
+    <t>28. Message-Door Held Open</t>
+  </si>
+  <si>
+    <t>29. Message-Card Granted</t>
+  </si>
+  <si>
+    <t>30. Message-Denied Card</t>
+  </si>
+  <si>
+    <t>31. Message-Denied start date</t>
+  </si>
+  <si>
+    <t>32. Message-Denied End date</t>
+  </si>
+  <si>
+    <t>Door VAX-1D Door is Now Locked</t>
+  </si>
+  <si>
+    <t>Door VAX Demo Door 1 is Now Open</t>
+  </si>
+  <si>
+    <t>Door VAX Demo Door 1 Is Being Held Open</t>
+  </si>
+  <si>
+    <t>Door VAX Demo Door 1 is Now Closed</t>
+  </si>
+  <si>
+    <t>Door VAX Demo Door 1 has been Forced Open</t>
+  </si>
+  <si>
+    <t>VAX Demo Door 2 has been overridden. Current state is Lockdown</t>
+  </si>
+  <si>
+    <t>VAX Demo Door 2 has resumed from an overridden state</t>
+  </si>
+  <si>
+    <t>VAX Demo Door 2 has been overridden. Current state is Unlock</t>
+  </si>
+  <si>
+    <t>Test VAX3.1 Granted Access to VAX Demo Door 1 Reader with credential 112-458</t>
+  </si>
+  <si>
+    <t>Test VAX3.1 granted access to VAX Demo Door 1 Reader due to master privilege with credential 112-458</t>
+  </si>
+  <si>
+    <t>demo Test demo Denied Access to VAX-1D Door Reader due to Invalid Time Zone with credential 115-1001</t>
+  </si>
+  <si>
+    <t>Unknown User Denied Access to VAX Demo Door 1 Reader due to Invalid Card or Pin with credential 115-1001</t>
+  </si>
+  <si>
+    <t>Test VAX3.1 Denied Access to VAX Demo Door 1 Reader due to Start Work Date with credential 112-458</t>
+  </si>
+  <si>
+    <t>Test VAX3.1 Denied Access to VAX Demo Door 1 Reader due to Expiry Date with credential 112-458</t>
+  </si>
+  <si>
+    <t>Test VAX3.1 Denied Access to VAX Demo Door 1 Reader. Users crisis level below doors current crisis level.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,11 +293,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,8 +588,8 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1"/>
     <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -476,12 +680,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A33E906-E1A3-4376-8BF8-9E10DB7D303B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{03AA13FA-F479-425A-A316-1A30F4EA91B2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -490,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91ECBCA9-56EE-4C8C-BE1F-5C0CE5A6028C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U16" sqref="U15:U16"/>
     </sheetView>
   </sheetViews>
@@ -510,4 +788,289 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AD6A25-A7A3-4FC9-8519-1A1F4584853C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D42274-6CB3-47C0-A091-D72F405B7FA2}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>